<commit_message>
minor modification in EIC
</commit_message>
<xml_diff>
--- a/EIC/expdata/3000.xlsx
+++ b/EIC/expdata/3000.xlsx
@@ -22,7 +22,7 @@
     <t>Eh</t>
   </si>
   <si>
-    <t>x</t>
+    <t>X</t>
   </si>
   <si>
     <t>Q2</t>
@@ -56,10 +56,10 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,29 +77,8 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -110,6 +89,30 @@
       <name val="Calibri Light"/>
       <charset val="134"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -128,9 +131,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -145,30 +170,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -181,21 +190,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -203,9 +197,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -220,7 +213,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -232,25 +231,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -274,7 +255,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -286,55 +273,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -352,7 +327,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -364,7 +339,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -376,31 +375,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,6 +404,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -425,6 +427,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -453,15 +464,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -473,15 +475,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -523,66 +516,66 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -920,7 +913,7 @@
   <dimension ref="A1:J391"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>

</xml_diff>